<commit_message>
Ajustes dos gráficos da dissertação.
</commit_message>
<xml_diff>
--- a/input/data_raw/64linhas.xlsx
+++ b/input/data_raw/64linhas.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b22ddafcbb9a5506/Documentos/DissertacaoUFF/input/data_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="8_{921A8998-F936-458A-A698-C68F69ACF9AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BBBC1823-BAA5-4F97-A1FD-F2275DA05690}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="8_{921A8998-F936-458A-A698-C68F69ACF9AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85C7F829-37BE-4345-8C79-21730BB585E6}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{30061EB9-BC1F-4F5D-BEDE-999D3DD71EB7}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{30061EB9-BC1F-4F5D-BEDE-999D3DD71EB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$D$1</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -453,6 +456,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -754,8 +761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F4C7802-6F7D-4D11-A7B7-2DDB5D4682D4}">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47:B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -782,112 +789,112 @@
     </row>
     <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
-        <v>388</v>
+        <v>104</v>
       </c>
       <c r="B2" s="4">
-        <v>388</v>
+        <v>104</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>1</v>
+        <v>77</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
-        <v>741</v>
+        <v>201</v>
       </c>
       <c r="B3" s="4">
-        <v>741</v>
+        <v>201</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>1</v>
+        <v>80</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="G3" s="9"/>
     </row>
     <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
-        <v>743</v>
+        <v>229</v>
       </c>
       <c r="B4" s="4">
-        <v>743</v>
+        <v>229</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>1</v>
+        <v>81</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
-        <v>808</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>3</v>
+        <v>254</v>
+      </c>
+      <c r="B5" s="4">
+        <v>254</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
-        <v>809</v>
+        <v>277</v>
       </c>
       <c r="B6" s="4">
-        <v>809</v>
+        <v>277</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
-        <v>822</v>
+        <v>311</v>
       </c>
       <c r="B7" s="4">
-        <v>822</v>
+        <v>311</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
-        <v>825</v>
+        <v>349</v>
       </c>
       <c r="B8" s="4">
-        <v>825</v>
+        <v>349</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
-        <v>830</v>
+        <v>388</v>
       </c>
       <c r="B9" s="4">
-        <v>830</v>
+        <v>388</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>1</v>
@@ -895,153 +902,153 @@
     </row>
     <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
-        <v>833</v>
+        <v>435</v>
       </c>
       <c r="B10" s="4">
-        <v>833</v>
+        <v>435</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>1</v>
+        <v>82</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
-        <v>842</v>
+        <v>448</v>
       </c>
       <c r="B11" s="4">
-        <v>842</v>
+        <v>448</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>1</v>
+        <v>83</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
-        <v>845</v>
+        <v>600</v>
       </c>
       <c r="B12" s="4">
-        <v>845</v>
+        <v>600</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>1</v>
+        <v>88</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
-        <v>849</v>
+        <v>603</v>
       </c>
       <c r="B13" s="4">
-        <v>849</v>
+        <v>603</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>1</v>
+        <v>89</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
-        <v>851</v>
+        <v>626</v>
       </c>
       <c r="B14" s="4">
-        <v>851</v>
+        <v>626</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>1</v>
+        <v>92</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
-        <v>870</v>
+        <v>651</v>
       </c>
       <c r="B15" s="4">
-        <v>870</v>
+        <v>651</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
-        <v>871</v>
+        <v>652</v>
       </c>
       <c r="B16" s="4">
-        <v>871</v>
+        <v>652</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
-        <v>885</v>
+        <v>669</v>
       </c>
       <c r="B17" s="4">
-        <v>885</v>
+        <v>669</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>16</v>
+        <v>55</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
-        <v>892</v>
+        <v>678</v>
       </c>
       <c r="B18" s="4">
-        <v>892</v>
+        <v>678</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4">
-        <v>893</v>
+        <v>709</v>
       </c>
       <c r="B19" s="4">
-        <v>893</v>
+        <v>709</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
-        <v>899</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>19</v>
+        <v>741</v>
+      </c>
+      <c r="B20" s="4">
+        <v>741</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>1</v>
@@ -1049,97 +1056,97 @@
     </row>
     <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4">
-        <v>651</v>
+        <v>743</v>
       </c>
       <c r="B21" s="4">
-        <v>651</v>
+        <v>743</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4">
-        <v>652</v>
+        <v>778</v>
       </c>
       <c r="B22" s="4">
-        <v>652</v>
+        <v>778</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4">
-        <v>678</v>
+        <v>809</v>
       </c>
       <c r="B23" s="4">
-        <v>678</v>
+        <v>809</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>25</v>
+      <c r="A24" s="4">
+        <v>822</v>
+      </c>
+      <c r="B24" s="4">
+        <v>822</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="4">
-        <v>702</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>27</v>
+        <v>825</v>
+      </c>
+      <c r="B25" s="4">
+        <v>825</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="4">
-        <v>709</v>
+        <v>830</v>
       </c>
       <c r="B26" s="4">
-        <v>709</v>
+        <v>830</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="4">
-        <v>785</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>30</v>
+        <v>831</v>
+      </c>
+      <c r="B27" s="4">
+        <v>831</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>22</v>
@@ -1147,83 +1154,83 @@
     </row>
     <row r="28" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="4">
-        <v>817</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>32</v>
+        <v>833</v>
+      </c>
+      <c r="B28" s="4">
+        <v>833</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="4">
-        <v>831</v>
+        <v>842</v>
       </c>
       <c r="B29" s="4">
-        <v>831</v>
+        <v>842</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>36</v>
+      <c r="A30" s="4">
+        <v>845</v>
+      </c>
+      <c r="B30" s="4">
+        <v>845</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="4">
-        <v>865</v>
+        <v>849</v>
       </c>
       <c r="B31" s="4">
-        <v>865</v>
+        <v>849</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="4">
-        <v>881</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>38</v>
+        <v>851</v>
+      </c>
+      <c r="B32" s="4">
+        <v>851</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="4">
-        <v>987</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>40</v>
+        <v>865</v>
+      </c>
+      <c r="B33" s="4">
+        <v>865</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>22</v>
@@ -1231,97 +1238,97 @@
     </row>
     <row r="34" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="4">
-        <v>990</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>42</v>
+        <v>870</v>
+      </c>
+      <c r="B34" s="4">
+        <v>870</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="4">
-        <v>254</v>
+        <v>871</v>
       </c>
       <c r="B35" s="4">
-        <v>254</v>
+        <v>871</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>45</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="4">
-        <v>277</v>
+        <v>885</v>
       </c>
       <c r="B36" s="4">
-        <v>277</v>
+        <v>885</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>45</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="4">
-        <v>311</v>
+        <v>892</v>
       </c>
       <c r="B37" s="4">
-        <v>311</v>
+        <v>892</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>45</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="4">
-        <v>349</v>
+        <v>893</v>
       </c>
       <c r="B38" s="4">
-        <v>349</v>
+        <v>893</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>45</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>50</v>
+      <c r="A39" s="4">
+        <v>901</v>
+      </c>
+      <c r="B39" s="4">
+        <v>901</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>53</v>
+      <c r="A40" s="4">
+        <v>915</v>
+      </c>
+      <c r="B40" s="4">
+        <v>915</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>45</v>
@@ -1329,41 +1336,41 @@
     </row>
     <row r="41" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="4">
-        <v>669</v>
+        <v>922</v>
       </c>
       <c r="B41" s="4">
-        <v>669</v>
+        <v>922</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>57</v>
+      <c r="A42" s="4">
+        <v>925</v>
+      </c>
+      <c r="B42" s="4">
+        <v>925</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>60</v>
+      <c r="A43" s="4">
+        <v>928</v>
+      </c>
+      <c r="B43" s="4">
+        <v>928</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>45</v>
@@ -1371,139 +1378,139 @@
     </row>
     <row r="44" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="4">
-        <v>778</v>
+        <v>951</v>
       </c>
       <c r="B44" s="4">
-        <v>778</v>
+        <v>951</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="4">
-        <v>901</v>
-      </c>
-      <c r="B45" s="4">
-        <v>901</v>
+      <c r="A45" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>69</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>45</v>
+        <v>70</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="4">
-        <v>915</v>
-      </c>
-      <c r="B46" s="4">
-        <v>915</v>
+      <c r="A46" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>75</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>45</v>
+        <v>76</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="4">
-        <v>922</v>
-      </c>
-      <c r="B47" s="4">
-        <v>922</v>
+        <v>817</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="4">
-        <v>925</v>
-      </c>
-      <c r="B48" s="4">
-        <v>925</v>
+        <v>881</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="4">
-        <v>928</v>
-      </c>
-      <c r="B49" s="4">
-        <v>928</v>
+        <v>990</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="4">
-        <v>951</v>
-      </c>
-      <c r="B50" s="4">
-        <v>951</v>
+        <v>987</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>69</v>
+      <c r="A51" s="4">
+        <v>808</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>71</v>
+        <v>4</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="B52" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C52" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>71</v>
+      <c r="A52" s="4">
+        <v>899</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>75</v>
+      <c r="A53" s="4">
+        <v>157</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>71</v>
@@ -1511,13 +1518,13 @@
     </row>
     <row r="54" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="4">
-        <v>104</v>
-      </c>
-      <c r="B54" s="4">
-        <v>104</v>
+        <v>605</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>90</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>71</v>
@@ -1525,41 +1532,41 @@
     </row>
     <row r="55" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="4">
-        <v>157</v>
+        <v>785</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>78</v>
+        <v>30</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>71</v>
+        <v>31</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="4">
-        <v>201</v>
-      </c>
-      <c r="B56" s="4">
-        <v>201</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D56" s="3" t="s">
+      <c r="A56" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D56" s="8" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="4">
-        <v>229</v>
-      </c>
-      <c r="B57" s="4">
-        <v>229</v>
+        <v>519</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>71</v>
@@ -1567,13 +1574,13 @@
     </row>
     <row r="58" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="4">
-        <v>435</v>
-      </c>
-      <c r="B58" s="4">
-        <v>435</v>
+        <v>518</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>84</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>71</v>
@@ -1581,103 +1588,108 @@
     </row>
     <row r="59" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="4">
-        <v>448</v>
-      </c>
-      <c r="B59" s="4">
-        <v>448</v>
+        <v>702</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>71</v>
+        <v>28</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="4">
-        <v>518</v>
+      <c r="A60" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>84</v>
+        <v>57</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>71</v>
+        <v>58</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="4">
-        <v>519</v>
+      <c r="A61" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>86</v>
+        <v>25</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>71</v>
+        <v>26</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="4">
-        <v>600</v>
-      </c>
-      <c r="B62" s="4">
-        <v>600</v>
+      <c r="A62" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>71</v>
+        <v>34</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="4">
-        <v>603</v>
-      </c>
-      <c r="B63" s="4">
-        <v>603</v>
+      <c r="A63" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>71</v>
+        <v>51</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="4">
-        <v>605</v>
+      <c r="A64" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>90</v>
+        <v>53</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>71</v>
+        <v>54</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="4">
-        <v>626</v>
-      </c>
-      <c r="B65" s="4">
-        <v>626</v>
+      <c r="A65" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>71</v>
+        <v>61</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D1" xr:uid="{7F4C7802-6F7D-4D11-A7B7-2DDB5D4682D4}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D65">
+      <sortCondition ref="B1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Criando cenário sugerido na banca de defessa da dissertação.
</commit_message>
<xml_diff>
--- a/input/data_raw/64linhas.xlsx
+++ b/input/data_raw/64linhas.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b22ddafcbb9a5506/Documentos/DissertacaoUFF/input/data_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="8_{921A8998-F936-458A-A698-C68F69ACF9AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85C7F829-37BE-4345-8C79-21730BB585E6}"/>
+  <xr:revisionPtr revIDLastSave="80" documentId="8_{921A8998-F936-458A-A698-C68F69ACF9AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{57359E1B-F5B9-4E54-8179-2ACA9ACEA903}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{30061EB9-BC1F-4F5D-BEDE-999D3DD71EB7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{30061EB9-BC1F-4F5D-BEDE-999D3DD71EB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$E$65</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="98">
   <si>
     <t>Cesarão X Candelária</t>
   </si>
@@ -330,6 +330,9 @@
   </si>
   <si>
     <t>consorcio</t>
+  </si>
+  <si>
+    <t>percent_cumprido</t>
   </si>
 </sst>
 </file>
@@ -761,8 +764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F4C7802-6F7D-4D11-A7B7-2DDB5D4682D4}">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47:B59"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -771,6 +774,7 @@
     <col min="2" max="2" width="16.88671875" style="2" customWidth="1"/>
     <col min="3" max="3" width="43.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -786,6 +790,9 @@
       <c r="D1" s="2" t="s">
         <v>96</v>
       </c>
+      <c r="E1" s="3" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
@@ -800,6 +807,9 @@
       <c r="D2" s="3" t="s">
         <v>71</v>
       </c>
+      <c r="E2">
+        <v>0.82789999999999997</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
@@ -814,6 +824,9 @@
       <c r="D3" s="3" t="s">
         <v>71</v>
       </c>
+      <c r="E3">
+        <v>0.746</v>
+      </c>
       <c r="G3" s="9"/>
     </row>
     <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -829,6 +842,9 @@
       <c r="D4" s="3" t="s">
         <v>71</v>
       </c>
+      <c r="E4">
+        <v>0.73140000000000005</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
@@ -843,6 +859,9 @@
       <c r="D5" s="2" t="s">
         <v>45</v>
       </c>
+      <c r="E5">
+        <v>0.68140000000000001</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
@@ -857,6 +876,9 @@
       <c r="D6" s="2" t="s">
         <v>45</v>
       </c>
+      <c r="E6">
+        <v>0.72750000000000004</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
@@ -871,6 +893,9 @@
       <c r="D7" s="2" t="s">
         <v>45</v>
       </c>
+      <c r="E7">
+        <v>0.63839999999999997</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
@@ -885,6 +910,9 @@
       <c r="D8" s="2" t="s">
         <v>45</v>
       </c>
+      <c r="E8">
+        <v>0.61040000000000005</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
@@ -899,6 +927,9 @@
       <c r="D9" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="E9">
+        <v>0.39639999999999997</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
@@ -913,6 +944,9 @@
       <c r="D10" s="3" t="s">
         <v>71</v>
       </c>
+      <c r="E10">
+        <v>0.56110000000000004</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
@@ -927,6 +961,9 @@
       <c r="D11" s="3" t="s">
         <v>71</v>
       </c>
+      <c r="E11">
+        <v>0.95379999999999998</v>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
@@ -941,6 +978,9 @@
       <c r="D12" s="3" t="s">
         <v>71</v>
       </c>
+      <c r="E12">
+        <v>0.99519999999999997</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
@@ -955,6 +995,9 @@
       <c r="D13" s="3" t="s">
         <v>71</v>
       </c>
+      <c r="E13">
+        <v>0.995</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
@@ -969,6 +1012,9 @@
       <c r="D14" s="3" t="s">
         <v>71</v>
       </c>
+      <c r="E14">
+        <v>0.78600000000000003</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
@@ -983,6 +1029,9 @@
       <c r="D15" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="E15">
+        <v>0.86960000000000004</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
@@ -997,8 +1046,11 @@
       <c r="D16" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E16">
+        <v>0.8911</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
         <v>669</v>
       </c>
@@ -1011,8 +1063,11 @@
       <c r="D17" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E17">
+        <v>0.81640000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
         <v>678</v>
       </c>
@@ -1025,8 +1080,11 @@
       <c r="D18" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E18">
+        <v>0.6673</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4">
         <v>709</v>
       </c>
@@ -1039,8 +1097,11 @@
       <c r="D19" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E19">
+        <v>0.19209999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
         <v>741</v>
       </c>
@@ -1053,8 +1114,11 @@
       <c r="D20" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E20">
+        <v>0.75700000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4">
         <v>743</v>
       </c>
@@ -1067,8 +1131,11 @@
       <c r="D21" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E21">
+        <v>0.76319999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4">
         <v>778</v>
       </c>
@@ -1081,8 +1148,11 @@
       <c r="D22" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E22">
+        <v>0.88780000000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4">
         <v>809</v>
       </c>
@@ -1095,8 +1165,11 @@
       <c r="D23" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E23">
+        <v>0.84279999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4">
         <v>822</v>
       </c>
@@ -1109,8 +1182,11 @@
       <c r="D24" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E24">
+        <v>0.88370000000000004</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="4">
         <v>825</v>
       </c>
@@ -1123,8 +1199,11 @@
       <c r="D25" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E25">
+        <v>0.65839999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="4">
         <v>830</v>
       </c>
@@ -1137,8 +1216,11 @@
       <c r="D26" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E26">
+        <v>0.61119999999999997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="4">
         <v>831</v>
       </c>
@@ -1151,8 +1233,11 @@
       <c r="D27" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E27">
+        <v>0.4919</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="4">
         <v>833</v>
       </c>
@@ -1165,8 +1250,11 @@
       <c r="D28" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E28">
+        <v>0.67259999999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="4">
         <v>842</v>
       </c>
@@ -1179,8 +1267,11 @@
       <c r="D29" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E29">
+        <v>0.57199999999999995</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="4">
         <v>845</v>
       </c>
@@ -1193,8 +1284,11 @@
       <c r="D30" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E30">
+        <v>0.95230000000000004</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="4">
         <v>849</v>
       </c>
@@ -1207,8 +1301,11 @@
       <c r="D31" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E31">
+        <v>0.8014</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="4">
         <v>851</v>
       </c>
@@ -1221,8 +1318,11 @@
       <c r="D32" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E32">
+        <v>0.93620000000000003</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="4">
         <v>865</v>
       </c>
@@ -1235,8 +1335,11 @@
       <c r="D33" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E33">
+        <v>0.3846</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="4">
         <v>870</v>
       </c>
@@ -1249,8 +1352,11 @@
       <c r="D34" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E34">
+        <v>0.94820000000000004</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="4">
         <v>871</v>
       </c>
@@ -1263,8 +1369,11 @@
       <c r="D35" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E35">
+        <v>0.80069999999999997</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="4">
         <v>885</v>
       </c>
@@ -1277,8 +1386,11 @@
       <c r="D36" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E36">
+        <v>0.78510000000000002</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="4">
         <v>892</v>
       </c>
@@ -1291,8 +1403,11 @@
       <c r="D37" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E37">
+        <v>0.77990000000000004</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="4">
         <v>893</v>
       </c>
@@ -1305,8 +1420,11 @@
       <c r="D38" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E38">
+        <v>0.87519999999999998</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="4">
         <v>901</v>
       </c>
@@ -1319,8 +1437,11 @@
       <c r="D39" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E39">
+        <v>0.57899999999999996</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="4">
         <v>915</v>
       </c>
@@ -1333,8 +1454,11 @@
       <c r="D40" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E40">
+        <v>0.106</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="4">
         <v>922</v>
       </c>
@@ -1347,8 +1471,11 @@
       <c r="D41" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E41">
+        <v>0.29409999999999997</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="4">
         <v>925</v>
       </c>
@@ -1361,8 +1488,11 @@
       <c r="D42" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E42">
+        <v>0.47989999999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="4">
         <v>928</v>
       </c>
@@ -1375,8 +1505,11 @@
       <c r="D43" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E43">
+        <v>1.0294000000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="4">
         <v>951</v>
       </c>
@@ -1389,8 +1522,11 @@
       <c r="D44" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E44">
+        <v>0.98509999999999998</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="5" t="s">
         <v>69</v>
       </c>
@@ -1403,8 +1539,11 @@
       <c r="D45" s="3" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E45">
+        <v>0.89970000000000006</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
         <v>75</v>
       </c>
@@ -1417,8 +1556,11 @@
       <c r="D46" s="3" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E46">
+        <v>0.89419999999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="4">
         <v>817</v>
       </c>
@@ -1431,8 +1573,11 @@
       <c r="D47" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E47">
+        <v>0.41760000000000003</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="4">
         <v>881</v>
       </c>
@@ -1445,8 +1590,11 @@
       <c r="D48" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E48">
+        <v>0.78710000000000002</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="4">
         <v>990</v>
       </c>
@@ -1459,8 +1607,11 @@
       <c r="D49" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E49">
+        <v>0.79559999999999997</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="4">
         <v>987</v>
       </c>
@@ -1473,8 +1624,11 @@
       <c r="D50" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E50">
+        <v>0.51449999999999996</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="4">
         <v>808</v>
       </c>
@@ -1487,8 +1641,11 @@
       <c r="D51" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E51">
+        <v>0.72909999999999997</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="4">
         <v>899</v>
       </c>
@@ -1501,8 +1658,11 @@
       <c r="D52" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E52">
+        <v>0.6109</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="4">
         <v>157</v>
       </c>
@@ -1515,8 +1675,11 @@
       <c r="D53" s="3" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E53">
+        <v>0.94110000000000005</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="4">
         <v>605</v>
       </c>
@@ -1529,8 +1692,11 @@
       <c r="D54" s="3" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E54">
+        <v>0.55689999999999995</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="4">
         <v>785</v>
       </c>
@@ -1543,8 +1709,11 @@
       <c r="D55" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E55">
+        <v>0.69279999999999997</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="7" t="s">
         <v>72</v>
       </c>
@@ -1557,8 +1726,11 @@
       <c r="D56" s="8" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E56">
+        <v>7.5800000000000006E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="4">
         <v>519</v>
       </c>
@@ -1571,8 +1743,11 @@
       <c r="D57" s="3" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E57">
+        <v>0.58199999999999996</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="4">
         <v>518</v>
       </c>
@@ -1585,8 +1760,11 @@
       <c r="D58" s="3" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E58">
+        <v>0.55740000000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="4">
         <v>702</v>
       </c>
@@ -1599,8 +1777,11 @@
       <c r="D59" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="4" t="s">
         <v>56</v>
       </c>
@@ -1613,8 +1794,11 @@
       <c r="D60" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E60">
+        <v>0.45440000000000003</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="4" t="s">
         <v>24</v>
       </c>
@@ -1627,8 +1811,11 @@
       <c r="D61" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E61">
+        <v>0.72070000000000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="4" t="s">
         <v>35</v>
       </c>
@@ -1641,8 +1828,11 @@
       <c r="D62" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E62">
+        <v>0.98699999999999999</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="4" t="s">
         <v>49</v>
       </c>
@@ -1655,8 +1845,11 @@
       <c r="D63" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E63">
+        <v>0.77310000000000001</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="4" t="s">
         <v>52</v>
       </c>
@@ -1669,8 +1862,11 @@
       <c r="D64" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E64">
+        <v>0.9083</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="4" t="s">
         <v>59</v>
       </c>
@@ -1683,13 +1879,11 @@
       <c r="D65" s="2" t="s">
         <v>45</v>
       </c>
+      <c r="E65">
+        <v>0.17369999999999999</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D1" xr:uid="{7F4C7802-6F7D-4D11-A7B7-2DDB5D4682D4}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D65">
-      <sortCondition ref="B1"/>
-    </sortState>
-  </autoFilter>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>